<commit_message>
added fake scpsch assisted, check test, and ingress test
</commit_message>
<xml_diff>
--- a/tests/fake_data/combined_scp_ch_fake.xlsx
+++ b/tests/fake_data/combined_scp_ch_fake.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eschdata\Strategic_Resourcing_CS$\Performance Improvement Team\Data to Insight\Will\903data\SCP CH data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FDA273-21CA-447A-B150-4F3DC04E2446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A968D679-B49D-4E5C-B9D6-07C24AA48390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3A5F04AB-1BB0-4216-8944-3B82FE5BB4B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A5F04AB-1BB0-4216-8944-3B82FE5BB4B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Providers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -772,7 +772,7 @@
   <dimension ref="A1:CV5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>